<commit_message>
exporta tablas a txt
</commit_message>
<xml_diff>
--- a/programacion/mauro/obligaciones_mauro.xlsx
+++ b/programacion/mauro/obligaciones_mauro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mauro\repos\ort\obligatorios\programacion\mauro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD6253F-CAB5-4AFA-9D72-75C4FF91DF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C05C782-6BDB-4C5B-9950-C1EC3BD61585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -524,7 +524,7 @@
   <dimension ref="A1:ER958"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2336,7 +2336,9 @@
       <c r="B19" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -2488,7 +2490,9 @@
       <c r="B20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -2640,7 +2644,9 @@
       <c r="B21" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="11"/>
+      <c r="C21" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -2792,7 +2798,9 @@
       <c r="B22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="11"/>
+      <c r="C22" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -2944,7 +2952,9 @@
       <c r="B23" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="11"/>
+      <c r="C23" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -3096,7 +3106,9 @@
       <c r="B24" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="14"/>
+      <c r="C24" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>

</xml_diff>